<commit_message>
feat: "Test 10 testcases and fix capacity random"
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -456,11 +456,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>(1,2, p = 15, c = 500)</t>
+          <t>(1,2, p = 13, c = 700)</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -472,11 +472,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>(1,4, p = 17, c = 200)</t>
+          <t>(1,4, p = 1, c = 133)</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -488,11 +488,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>(2,3, p = 8, c = 100)</t>
+          <t>(2,3, p = 10, c = 600)</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -504,11 +504,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>(2,5, p = 7, c = 133)</t>
+          <t>(2,5, p = 16, c = 200)</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -520,11 +520,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>(3,6, p = 12, c = 100)</t>
+          <t>(3,6, p = 9, c = 200)</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -536,11 +536,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>(4,5, p = 15, c = 700)</t>
+          <t>(4,5, p = 10, c = 500)</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -552,11 +552,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>(4,7, p = 1, c = 500)</t>
+          <t>(4,7, p = 14, c = 200)</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -568,11 +568,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>(5,6, p = 5, c = 200)</t>
+          <t>(5,6, p = 19, c = 700)</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -584,11 +584,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>(5,8, p = 7, c = 500)</t>
+          <t>(5,8, p = 4, c = 500)</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D10" t="n">
         <v>-400</v>

</xml_diff>